<commit_message>
se genera el pdf
</commit_message>
<xml_diff>
--- a/ejemplo.xlsx
+++ b/ejemplo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>userName</t>
   </si>
@@ -28,10 +28,10 @@
     <t>endTime</t>
   </si>
   <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>PRESENTE</t>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>FALTA</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -433,6 +433,14 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>